<commit_message>
two questions are added is marksheet
</commit_message>
<xml_diff>
--- a/marksheet.xlsx
+++ b/marksheet.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Database" sheetId="1" r:id="rId1"/>
+    <sheet name="Query" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="312">
   <si>
     <t>student_id</t>
   </si>
@@ -946,13 +947,22 @@
   </si>
   <si>
     <t>Rory DuBuque</t>
+  </si>
+  <si>
+    <t>Find name from student_id (first_name)</t>
+  </si>
+  <si>
+    <t>Find name from student_id (first_name and last_name)</t>
+  </si>
+  <si>
+    <t>Solve the following problems</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -966,8 +976,30 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -977,6 +1009,23 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -989,15 +1038,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
+    <cellStyle name="20% - Accent5" xfId="3" builtinId="46"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1279,8 +1344,8 @@
   </sheetPr>
   <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,6 +1358,9 @@
     <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="16" max="16" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5676,5 +5744,94 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15:F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="4" spans="4:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>19359</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="10" spans="4:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D10" s="4">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="7"/>
+      <c r="G13" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="E10:K10"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>